<commit_message>
Updated C3DC phs002371 queries
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs002371_SexAtBirth-Male.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs002371_SexAtBirth-Male.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECA59AD-8DC9-5F44-98DE-0B9603AD6BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD28918-3F90-254E-87A5-95AF64EE965E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,6 +226,41 @@
   <si>
     <t>SELECT DISTINCT
     prt.participant_id AS "Participant Id",
+    srv.survival_id AS "Survival Id",
+    srv.last_known_survival_status AS "Last Known Survival Status",
+    CASE 
+    WHEN srv.age_at_last_known_survival_status = -999 THEN 'Not Reported'
+    WHEN srv.age_at_last_known_survival_status &gt;= 1000 THEN 
+        substr(srv.age_at_last_known_survival_status, 1, length(srv.age_at_last_known_survival_status) - 3) || ',' || substr(srv.age_at_last_known_survival_status, -3)
+    ELSE 
+        srv.age_at_last_known_survival_status 
+END AS "Age at Last Known Survival Status",
+    srv.first_event AS "First Event",
+    srv.cause_of_death AS "Cause of Death",
+    std.dbgap_accession AS "dbGaP Accession"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnoses dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_treatments trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+LEFT JOIN 
+    df_reference_files rfs ON std.id = rfs."study.id"
+WHERE 
+    std.dbgap_accession = 'phs002371' AND prt.sex_at_birth = 'Male' AND srv.survival_id IS NOT NULL
+ORDER BY 
+    prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant Id",
     trr.treatment_response_id AS "Treatment Response Id",
     trr.response AS "Response",
     CASE 
@@ -253,42 +288,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs002371' AND prt.sex_at_birth = 'Male'
-ORDER BY 
-    prt.participant_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    prt.participant_id AS "Participant Id",
-    srv.survival_id AS "Survival Id",
-    srv.last_known_survival_status AS "Last Known Survival Status",
-    CASE 
-    WHEN srv.age_at_last_known_survival_status = -999 THEN 'Not Reported'
-    WHEN srv.age_at_last_known_survival_status &gt;= 1000 THEN 
-        substr(srv.age_at_last_known_survival_status, 1, length(srv.age_at_last_known_survival_status) - 3) || ',' || substr(srv.age_at_last_known_survival_status, -3)
-    ELSE 
-        srv.age_at_last_known_survival_status 
-END AS "Age at Last Known Survival Status",
-    srv.first_event AS "First Event",
-    srv.cause_of_death AS "Cause of Death",
-    std.dbgap_accession AS "dbGaP Accession"
-FROM 
-    df_study std
-LEFT JOIN 
-    df_participant prt ON std.id = prt."study.id"
-LEFT JOIN 
-    df_diagnoses dgn ON prt.id = dgn."participant.id"
-LEFT JOIN 
-    df_treatments trt ON prt.id = trt."participant.id"
-LEFT JOIN 
-    df_treatment_resp trr ON prt.id = trr."participant.id"
-LEFT JOIN 
-    df_survival srv ON prt.id = srv."participant.id"
-LEFT JOIN 
-    df_reference_files rfs ON std.id = rfs."study.id"
-WHERE 
-    std.dbgap_accession = 'phs002371' AND prt.sex_at_birth = 'Male' AND srv.survival_id IS NOT NULL
+    std.dbgap_accession = 'phs002371' AND prt.sex_at_birth = 'Male' AND trt.treatment_id IS NOT NULL
 ORDER BY 
     prt.participant_id ASC
 LIMIT 100;</t>
@@ -298,9 +298,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -353,11 +360,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -684,7 +694,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -760,8 +770,8 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>18</v>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="2"/>
     </row>
@@ -770,7 +780,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -782,7 +792,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>